<commit_message>
Added assembly details for V3 of the PCB
</commit_message>
<xml_diff>
--- a/Qwiic_Iridium_9603N_BOM.xlsx
+++ b/Qwiic_Iridium_9603N_BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\thunderbird\home\pclark\Documents\eagle\SparkFun_Qwiic_Iridium_9603N\V3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Qwiic_Iridium_9603N\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="202">
   <si>
     <t>X</t>
   </si>
@@ -1494,9 +1494,7 @@
   </sheetPr>
   <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1975,21 +1973,21 @@
         <v>66</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>140</v>
+        <v>68</v>
+      </c>
+      <c r="I19" s="9">
+        <v>2496916</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6" t="s">
-        <v>141</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>